<commit_message>
Added in a CPI and APR chart with data drawn from BLS.
</commit_message>
<xml_diff>
--- a/US_Housing_Macro_Analysis.xlsx
+++ b/US_Housing_Macro_Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryanandrade/Desktop/GitHub/US_Housing_Macro/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77981CB5-A4C5-6F40-B642-5CEC49FD1A7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5534DE2-2ABF-A147-8B91-737EFA308A8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="34560" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="2" xr2:uid="{3A49B0E1-5FA0-8044-98A4-BAD0FA39CA68}"/>
   </bookViews>
@@ -138,13 +138,13 @@
     <t>% Loss</t>
   </si>
   <si>
-    <t>Years of Gain</t>
-  </si>
-  <si>
     <t>% Gain</t>
   </si>
   <si>
-    <t>Years of Loss</t>
+    <t>Years of Expansion</t>
+  </si>
+  <si>
+    <t>Years of Recession</t>
   </si>
 </sst>
 </file>
@@ -5889,19 +5889,19 @@
   <dimension ref="A1:I64"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="18.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="6.1640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
@@ -5932,10 +5932,10 @@
         <v>18</v>
       </c>
       <c r="D5" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="24" t="s">
         <v>25</v>
-      </c>
-      <c r="E5" s="24" t="s">
-        <v>26</v>
       </c>
       <c r="F5" s="25" t="s">
         <v>22</v>
@@ -5965,6 +5965,9 @@
       <c r="D6">
         <v>0</v>
       </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="12">
@@ -5976,6 +5979,9 @@
       <c r="C7" s="22">
         <v>11.5825</v>
       </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="12">
@@ -5986,6 +5992,15 @@
       </c>
       <c r="C8" s="22">
         <v>12.362500000000001</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="F8">
+        <v>1965</v>
+      </c>
+      <c r="G8">
+        <v>1966</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -6617,7 +6632,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{559305EB-3C1A-684E-B80A-B5582192B003}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0"/>
+    <sheetView topLeftCell="A7" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData/>

</xml_diff>

<commit_message>
Completed automation of housing sales revenue.
</commit_message>
<xml_diff>
--- a/US_Housing_Macro_Analysis.xlsx
+++ b/US_Housing_Macro_Analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryanandrade/Desktop/GitHub/US_Housing_Macro/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE2A974F-75A5-0948-A5BB-E6B0FE1C04EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9068181C-43CF-504E-A651-C6CBDC6FDAC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-160" yWindow="760" windowWidth="34560" windowHeight="19680" activeTab="2" xr2:uid="{3A49B0E1-5FA0-8044-98A4-BAD0FA39CA68}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19680" activeTab="2" xr2:uid="{3A49B0E1-5FA0-8044-98A4-BAD0FA39CA68}"/>
   </bookViews>
   <sheets>
     <sheet name="# Sold" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
   <si>
     <t>Houses Sold by Region</t>
   </si>
@@ -135,12 +135,6 @@
     <t>Valley</t>
   </si>
   <si>
-    <t>% Loss</t>
-  </si>
-  <si>
-    <t>% Gain</t>
-  </si>
-  <si>
     <t>Period of Expansion</t>
   </si>
   <si>
@@ -155,6 +149,9 @@
   <si>
     <t>Sales</t>
   </si>
+  <si>
+    <t>% Change</t>
+  </si>
 </sst>
 </file>
 
@@ -164,7 +161,7 @@
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
     <numFmt numFmtId="165" formatCode="mmm\ yyyy"/>
-    <numFmt numFmtId="167" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -388,6 +385,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -406,7 +404,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -3561,17 +3558,17 @@
       <c r="F3" s="2"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="19"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="21" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -3583,7 +3580,7 @@
       <c r="F6" s="4"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="21"/>
+      <c r="A7" s="22"/>
       <c r="B7" s="5" t="s">
         <v>5</v>
       </c>
@@ -3593,9 +3590,9 @@
       <c r="F7" s="5"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="21"/>
+      <c r="A8" s="22"/>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>6</v>
@@ -3614,9 +3611,9 @@
       </c>
     </row>
     <row r="9" spans="1:9" ht="13.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="22"/>
+      <c r="A9" s="23"/>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>11</v>
@@ -5233,18 +5230,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
     </row>
     <row r="4" spans="1:3" ht="13.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="5" spans="1:3" ht="24.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -5936,10 +5933,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A7966E2-C3F6-724E-A5A0-D24726136052}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:H64"/>
+  <dimension ref="A1:G64"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5947,142 +5944,138 @@
     <col min="2" max="2" width="22.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="17.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
       <c r="D1" s="16" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="24" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-    </row>
-    <row r="5" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+    </row>
+    <row r="5" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="18" t="s">
         <v>22</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>29</v>
       </c>
       <c r="F5" s="18" t="s">
         <v>23</v>
       </c>
       <c r="G5" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="H5" s="17" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="8">
         <v>1963</v>
       </c>
-      <c r="B6" s="25" cm="1">
+      <c r="B6" s="19" cm="1">
         <f t="array" ref="B6:B64">'# Sold'!B10:B68 *'Average Price'!C6:C64</f>
         <v>10808000000</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="8">
         <v>1964</v>
       </c>
-      <c r="B7" s="25">
+      <c r="B7" s="19">
         <v>11582500000</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="8">
         <v>1965</v>
       </c>
-      <c r="B8" s="25">
+      <c r="B8" s="19">
         <v>12362500000</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="8">
         <v>1966</v>
       </c>
-      <c r="B9" s="25">
+      <c r="B9" s="19">
         <v>10741300000</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="8">
         <v>1967</v>
       </c>
-      <c r="B10" s="25">
+      <c r="B10" s="19">
         <v>11980200000</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="8">
         <v>1968</v>
       </c>
-      <c r="B11" s="25">
+      <c r="B11" s="19">
         <v>13034000000</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="8">
         <v>1969</v>
       </c>
-      <c r="B12" s="25">
+      <c r="B12" s="19">
         <v>12499200000</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="8">
         <v>1970</v>
       </c>
-      <c r="B13" s="25">
+      <c r="B13" s="19">
         <v>12901000000</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="8">
         <v>1971</v>
       </c>
-      <c r="B14" s="25">
+      <c r="B14" s="19">
         <v>18564800000</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="8">
         <v>1972</v>
       </c>
-      <c r="B15" s="25">
+      <c r="B15" s="19">
         <v>21899000000</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="8">
         <v>1973</v>
       </c>
-      <c r="B16" s="25">
+      <c r="B16" s="19">
         <v>22507000000</v>
       </c>
     </row>
@@ -6090,7 +6083,7 @@
       <c r="A17" s="8">
         <v>1974</v>
       </c>
-      <c r="B17" s="25">
+      <c r="B17" s="19">
         <v>20189100000</v>
       </c>
     </row>
@@ -6098,7 +6091,7 @@
       <c r="A18" s="8">
         <v>1975</v>
       </c>
-      <c r="B18" s="25">
+      <c r="B18" s="19">
         <v>23387400000</v>
       </c>
     </row>
@@ -6106,7 +6099,7 @@
       <c r="A19" s="8">
         <v>1976</v>
       </c>
-      <c r="B19" s="25">
+      <c r="B19" s="19">
         <v>31008000000</v>
       </c>
     </row>
@@ -6114,7 +6107,7 @@
       <c r="A20" s="8">
         <v>1977</v>
       </c>
-      <c r="B20" s="25">
+      <c r="B20" s="19">
         <v>44389800000</v>
       </c>
     </row>
@@ -6122,7 +6115,7 @@
       <c r="A21" s="8">
         <v>1978</v>
       </c>
-      <c r="B21" s="25">
+      <c r="B21" s="19">
         <v>51062500000</v>
       </c>
     </row>
@@ -6130,7 +6123,7 @@
       <c r="A22" s="8">
         <v>1979</v>
       </c>
-      <c r="B22" s="25">
+      <c r="B22" s="19">
         <v>50906200000</v>
       </c>
     </row>
@@ -6138,7 +6131,7 @@
       <c r="A23" s="8">
         <v>1980</v>
       </c>
-      <c r="B23" s="25">
+      <c r="B23" s="19">
         <v>41638000000</v>
       </c>
     </row>
@@ -6146,7 +6139,7 @@
       <c r="A24" s="8">
         <v>1981</v>
       </c>
-      <c r="B24" s="25">
+      <c r="B24" s="19">
         <v>36188000000</v>
       </c>
     </row>
@@ -6154,7 +6147,7 @@
       <c r="A25" s="8">
         <v>1982</v>
       </c>
-      <c r="B25" s="25">
+      <c r="B25" s="19">
         <v>34566800000</v>
       </c>
     </row>
@@ -6162,7 +6155,7 @@
       <c r="A26" s="8">
         <v>1983</v>
       </c>
-      <c r="B26" s="25">
+      <c r="B26" s="19">
         <v>55945400000</v>
       </c>
     </row>
@@ -6170,7 +6163,7 @@
       <c r="A27" s="8">
         <v>1984</v>
       </c>
-      <c r="B27" s="25">
+      <c r="B27" s="19">
         <v>62366400000</v>
       </c>
     </row>
@@ -6178,7 +6171,7 @@
       <c r="A28" s="8">
         <v>1985</v>
       </c>
-      <c r="B28" s="25">
+      <c r="B28" s="19">
         <v>69350400000</v>
       </c>
     </row>
@@ -6186,7 +6179,7 @@
       <c r="A29" s="8">
         <v>1986</v>
       </c>
-      <c r="B29" s="25">
+      <c r="B29" s="19">
         <v>83925000000</v>
       </c>
     </row>
@@ -6194,7 +6187,7 @@
       <c r="A30" s="8">
         <v>1987</v>
       </c>
-      <c r="B30" s="25">
+      <c r="B30" s="19">
         <v>85351200000</v>
       </c>
     </row>
@@ -6202,7 +6195,7 @@
       <c r="A31" s="8">
         <v>1988</v>
       </c>
-      <c r="B31" s="25">
+      <c r="B31" s="19">
         <v>93490800000</v>
       </c>
     </row>
@@ -6210,7 +6203,7 @@
       <c r="A32" s="8">
         <v>1989</v>
       </c>
-      <c r="B32" s="25">
+      <c r="B32" s="19">
         <v>96720000000</v>
       </c>
     </row>
@@ -6218,7 +6211,7 @@
       <c r="A33" s="8">
         <v>1990</v>
       </c>
-      <c r="B33" s="25">
+      <c r="B33" s="19">
         <v>79993200000</v>
       </c>
     </row>
@@ -6226,7 +6219,7 @@
       <c r="A34" s="8">
         <v>1991</v>
       </c>
-      <c r="B34" s="25">
+      <c r="B34" s="19">
         <v>74924800000</v>
       </c>
     </row>
@@ -6234,7 +6227,7 @@
       <c r="A35" s="8">
         <v>1992</v>
       </c>
-      <c r="B35" s="25">
+      <c r="B35" s="19">
         <v>87901000000</v>
       </c>
     </row>
@@ -6242,7 +6235,7 @@
       <c r="A36" s="8">
         <v>1993</v>
       </c>
-      <c r="B36" s="25">
+      <c r="B36" s="19">
         <v>98368200000</v>
       </c>
     </row>
@@ -6250,7 +6243,7 @@
       <c r="A37" s="8">
         <v>1994</v>
       </c>
-      <c r="B37" s="25">
+      <c r="B37" s="19">
         <v>103515000000</v>
       </c>
     </row>
@@ -6258,7 +6251,7 @@
       <c r="A38" s="8">
         <v>1995</v>
       </c>
-      <c r="B38" s="25">
+      <c r="B38" s="19">
         <v>105852900000</v>
       </c>
     </row>
@@ -6266,7 +6259,7 @@
       <c r="A39" s="8">
         <v>1996</v>
       </c>
-      <c r="B39" s="25">
+      <c r="B39" s="19">
         <v>125964800000</v>
       </c>
     </row>
@@ -6274,7 +6267,7 @@
       <c r="A40" s="8">
         <v>1997</v>
       </c>
-      <c r="B40" s="25">
+      <c r="B40" s="19">
         <v>141664800000</v>
       </c>
     </row>
@@ -6282,7 +6275,7 @@
       <c r="A41" s="8">
         <v>1998</v>
       </c>
-      <c r="B41" s="25">
+      <c r="B41" s="19">
         <v>161163400000</v>
       </c>
     </row>
@@ -6290,7 +6283,7 @@
       <c r="A42" s="8">
         <v>1999</v>
       </c>
-      <c r="B42" s="25">
+      <c r="B42" s="19">
         <v>172128000000</v>
       </c>
     </row>
@@ -6298,7 +6291,7 @@
       <c r="A43" s="8">
         <v>2000</v>
       </c>
-      <c r="B43" s="25">
+      <c r="B43" s="19">
         <v>181539000000</v>
       </c>
     </row>
@@ -6306,7 +6299,7 @@
       <c r="A44" s="8">
         <v>2001</v>
       </c>
-      <c r="B44" s="25">
+      <c r="B44" s="19">
         <v>193585600000</v>
       </c>
     </row>
@@ -6314,7 +6307,7 @@
       <c r="A45" s="8">
         <v>2002</v>
       </c>
-      <c r="B45" s="25">
+      <c r="B45" s="19">
         <v>222525100000</v>
       </c>
     </row>
@@ -6322,7 +6315,7 @@
       <c r="A46" s="8">
         <v>2003</v>
       </c>
-      <c r="B46" s="25">
+      <c r="B46" s="19">
         <v>267481800000</v>
       </c>
     </row>
@@ -6330,7 +6323,7 @@
       <c r="A47" s="8">
         <v>2004</v>
       </c>
-      <c r="B47" s="25">
+      <c r="B47" s="19">
         <v>330223500000</v>
       </c>
     </row>
@@ -6338,7 +6331,7 @@
       <c r="A48" s="8">
         <v>2005</v>
       </c>
-      <c r="B48" s="25">
+      <c r="B48" s="19">
         <v>381051000000</v>
       </c>
     </row>
@@ -6346,7 +6339,7 @@
       <c r="A49" s="8">
         <v>2006</v>
       </c>
-      <c r="B49" s="25">
+      <c r="B49" s="19">
         <v>321500900000</v>
       </c>
     </row>
@@ -6354,7 +6347,7 @@
       <c r="A50" s="8">
         <v>2007</v>
       </c>
-      <c r="B50" s="25">
+      <c r="B50" s="19">
         <v>243353600000</v>
       </c>
     </row>
@@ -6362,7 +6355,7 @@
       <c r="A51" s="8">
         <v>2008</v>
       </c>
-      <c r="B51" s="25">
+      <c r="B51" s="19">
         <v>141911000000</v>
       </c>
     </row>
@@ -6370,7 +6363,7 @@
       <c r="A52" s="8">
         <v>2009</v>
       </c>
-      <c r="B52" s="25">
+      <c r="B52" s="19">
         <v>101587500000</v>
       </c>
     </row>
@@ -6378,7 +6371,7 @@
       <c r="A53" s="8">
         <v>2010</v>
       </c>
-      <c r="B53" s="25">
+      <c r="B53" s="19">
         <v>88146700000</v>
       </c>
     </row>
@@ -6386,7 +6379,7 @@
       <c r="A54" s="8">
         <v>2011</v>
       </c>
-      <c r="B54" s="25">
+      <c r="B54" s="19">
         <v>81977400000</v>
       </c>
     </row>
@@ -6394,7 +6387,7 @@
       <c r="A55" s="8">
         <v>2012</v>
       </c>
-      <c r="B55" s="25">
+      <c r="B55" s="19">
         <v>107529600000</v>
       </c>
     </row>
@@ -6402,7 +6395,7 @@
       <c r="A56" s="8">
         <v>2013</v>
       </c>
-      <c r="B56" s="25">
+      <c r="B56" s="19">
         <v>139210500000</v>
       </c>
     </row>
@@ -6410,7 +6403,7 @@
       <c r="A57" s="8">
         <v>2014</v>
       </c>
-      <c r="B57" s="25">
+      <c r="B57" s="19">
         <v>151944900000</v>
       </c>
     </row>
@@ -6418,7 +6411,7 @@
       <c r="A58" s="8">
         <v>2015</v>
       </c>
-      <c r="B58" s="25">
+      <c r="B58" s="19">
         <v>176702700000</v>
       </c>
     </row>
@@ -6426,7 +6419,7 @@
       <c r="A59" s="8">
         <v>2016</v>
       </c>
-      <c r="B59" s="25">
+      <c r="B59" s="19">
         <v>202464900000</v>
       </c>
     </row>
@@ -6434,7 +6427,7 @@
       <c r="A60" s="8">
         <v>2017</v>
       </c>
-      <c r="B60" s="25">
+      <c r="B60" s="19">
         <v>235943700000</v>
       </c>
     </row>
@@ -6442,7 +6435,7 @@
       <c r="A61" s="8">
         <v>2018</v>
       </c>
-      <c r="B61" s="25">
+      <c r="B61" s="19">
         <v>237545000000</v>
       </c>
     </row>
@@ -6450,7 +6443,7 @@
       <c r="A62" s="8">
         <v>2019</v>
       </c>
-      <c r="B62" s="25">
+      <c r="B62" s="19">
         <v>262203700000</v>
       </c>
     </row>
@@ -6458,7 +6451,7 @@
       <c r="A63" s="8">
         <v>2020</v>
       </c>
-      <c r="B63" s="25">
+      <c r="B63" s="19">
         <v>322141800000</v>
       </c>
     </row>
@@ -6466,7 +6459,7 @@
       <c r="A64" s="8">
         <v>2021</v>
       </c>
-      <c r="B64" s="25">
+      <c r="B64" s="19">
         <v>357898200000</v>
       </c>
     </row>

</xml_diff>